<commit_message>
Created new articles fixture
</commit_message>
<xml_diff>
--- a/products/fixtures/NX1.xlsx
+++ b/products/fixtures/NX1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djang\Documents\Soccersystems\products\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400C5179-F0D2-45D5-9A1F-922AAA35B4A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25AC3CB0-FC3E-4F64-A240-8AA704991BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="155">
   <si>
     <t>slug</t>
   </si>
@@ -97,9 +97,6 @@
     <t>NX10428W</t>
   </si>
   <si>
-    <t>NX10818W</t>
-  </si>
-  <si>
     <t>NX10824W</t>
   </si>
   <si>
@@ -163,12 +160,6 @@
     <t>NX1</t>
   </si>
   <si>
-    <t>ABN Amro logo (wit)</t>
-  </si>
-  <si>
-    <t>ABN Amro logo (zwart)</t>
-  </si>
-  <si>
     <t>Acronis (wit)</t>
   </si>
   <si>
@@ -184,27 +175,12 @@
     <t>Adidas &amp; Ziggo (wit)</t>
   </si>
   <si>
-    <t>Ajax logo (wit-goud)</t>
-  </si>
-  <si>
-    <t>Ajax logo (wit)</t>
-  </si>
-  <si>
-    <t>Ajax logo (zwart)</t>
-  </si>
-  <si>
     <t>Curacao (wit)</t>
   </si>
   <si>
     <t>Curacao (zwart)</t>
   </si>
   <si>
-    <t>Ziggo logo (wit)</t>
-  </si>
-  <si>
-    <t>Ziggo logo (zwart)</t>
-  </si>
-  <si>
     <t>NX10707B</t>
   </si>
   <si>
@@ -226,24 +202,9 @@
     <t>02036495</t>
   </si>
   <si>
-    <t>18075248</t>
-  </si>
-  <si>
-    <t>45859940</t>
-  </si>
-  <si>
-    <t>35674560</t>
-  </si>
-  <si>
-    <t>68277858</t>
-  </si>
-  <si>
     <t>NX10307Z</t>
   </si>
   <si>
-    <t>ABN Amro logo (331C)</t>
-  </si>
-  <si>
     <t>Acronis  (331C)</t>
   </si>
   <si>
@@ -307,9 +268,6 @@
     <t>articles/NX10428W.svg</t>
   </si>
   <si>
-    <t>articles/NX10818W.svg</t>
-  </si>
-  <si>
     <t>articles/NX10824W.svg</t>
   </si>
   <si>
@@ -397,9 +355,6 @@
     <t>articles/NX10205W.svg</t>
   </si>
   <si>
-    <t>49059947</t>
-  </si>
-  <si>
     <t>Curacao (331C)</t>
   </si>
   <si>
@@ -421,13 +376,115 @@
     <t>articles/NX10613B.svg</t>
   </si>
   <si>
-    <t>59785476</t>
-  </si>
-  <si>
     <t>01084079</t>
   </si>
   <si>
-    <t>97609392</t>
+    <t>NX10106V</t>
+  </si>
+  <si>
+    <t>NX10107V</t>
+  </si>
+  <si>
+    <t>NX10610Y</t>
+  </si>
+  <si>
+    <t>NX10613Y</t>
+  </si>
+  <si>
+    <t>NX10606Y</t>
+  </si>
+  <si>
+    <t>NX10221W</t>
+  </si>
+  <si>
+    <t>05202378</t>
+  </si>
+  <si>
+    <t>08047666</t>
+  </si>
+  <si>
+    <t>Acronis (331C)</t>
+  </si>
+  <si>
+    <t>Curacao (geel)</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>articles/NX10106V.svg</t>
+  </si>
+  <si>
+    <t>articles/NX10107V.svg</t>
+  </si>
+  <si>
+    <t>articles/NX10610Y.svg</t>
+  </si>
+  <si>
+    <t>articles/NX10613Y.svg</t>
+  </si>
+  <si>
+    <t>articles/NX10606Y.svg</t>
+  </si>
+  <si>
+    <t>articles/NX10221W.svg</t>
+  </si>
+  <si>
+    <t>ABN Amro (331C)</t>
+  </si>
+  <si>
+    <t>ABN Amro (wit)</t>
+  </si>
+  <si>
+    <t>ABN Amro (zwart)</t>
+  </si>
+  <si>
+    <t>Ajax (wit-goud)</t>
+  </si>
+  <si>
+    <t>Ajax (wit)</t>
+  </si>
+  <si>
+    <t>Ajax (zwart)</t>
+  </si>
+  <si>
+    <t>Ziggo (wit)</t>
+  </si>
+  <si>
+    <t>Ziggo (zwart)</t>
+  </si>
+  <si>
+    <t>Ajax (oud wit)</t>
   </si>
 </sst>
 </file>
@@ -474,7 +531,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -486,23 +543,17 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -806,9 +857,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -834,7 +887,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -858,525 +911,525 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" s="2">
         <v>4</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>71</v>
+      <c r="D2" s="8">
+        <v>45859940</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F2" s="9">
-        <v>7</v>
-      </c>
-      <c r="G2" s="5">
-        <v>0.28000000000000003</v>
+        <v>146</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G2" s="6">
+        <v>0.51</v>
       </c>
       <c r="H2" s="2">
         <v>0</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>75</v>
+      <c r="I2" s="7" t="s">
+        <v>69</v>
       </c>
       <c r="J2" s="3"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="2">
         <v>4</v>
       </c>
       <c r="D3" s="8">
-        <v>48255568</v>
+        <v>35674560</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" s="9">
-        <v>23</v>
-      </c>
-      <c r="G3" s="5">
-        <v>0.6</v>
+        <v>146</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0.72</v>
       </c>
       <c r="H3" s="2">
         <v>0</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>76</v>
+      <c r="I3" s="7" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="2">
         <v>4</v>
       </c>
       <c r="D4" s="8">
-        <v>13851562</v>
+        <v>18075248</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4" s="9">
-        <v>28</v>
-      </c>
-      <c r="G4" s="5">
-        <v>0.85</v>
+        <v>146</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0.24</v>
       </c>
       <c r="H4" s="2">
         <v>0</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>77</v>
+      <c r="I4" s="7" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>72</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" s="2">
         <v>4</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>65</v>
+      <c r="D5" s="8">
+        <v>48255568</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="9">
-        <v>7</v>
-      </c>
-      <c r="G5" s="5">
-        <v>0.28000000000000003</v>
+        <v>147</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0.51</v>
       </c>
       <c r="H5" s="2">
         <v>0</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>78</v>
+      <c r="I5" s="7" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6" s="2">
         <v>4</v>
       </c>
       <c r="D6" s="8">
-        <v>80270479</v>
+        <v>13851562</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" s="9">
-        <v>23</v>
-      </c>
-      <c r="G6" s="5">
-        <v>0.6</v>
+        <v>147</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0.72</v>
       </c>
       <c r="H6" s="2">
         <v>0</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>79</v>
+      <c r="I6" s="7" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C7" s="2">
         <v>4</v>
       </c>
       <c r="D7" s="8">
-        <v>53585604</v>
+        <v>68277858</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" s="9">
-        <v>28</v>
-      </c>
-      <c r="G7" s="5">
-        <v>0.85</v>
+        <v>147</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="G7" s="6">
+        <v>0.24</v>
       </c>
       <c r="H7" s="2">
         <v>0</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>80</v>
+      <c r="I7" s="7" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>62</v>
+        <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" s="2">
         <v>4</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>68</v>
+      <c r="D8" s="8">
+        <v>80270479</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F8" s="9">
-        <v>7</v>
-      </c>
-      <c r="G8" s="10">
-        <v>0.28000000000000003</v>
+        <v>148</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G8" s="6">
+        <v>0.51</v>
       </c>
       <c r="H8" s="2">
         <v>0</v>
       </c>
-      <c r="I8" s="2" t="s">
-        <v>81</v>
+      <c r="I8" s="7" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9" s="2">
         <v>4</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>69</v>
+      <c r="D9" s="8">
+        <v>53585604</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F9" s="9">
-        <v>23</v>
-      </c>
-      <c r="G9" s="10">
-        <v>0.6</v>
+        <v>148</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0.72</v>
       </c>
       <c r="H9" s="2">
         <v>0</v>
       </c>
-      <c r="I9" s="2" t="s">
-        <v>82</v>
+      <c r="I9" s="7" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" s="2">
         <v>4</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F10" s="9">
-        <v>28</v>
-      </c>
-      <c r="G10" s="10">
-        <v>0.85</v>
+        <v>148</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0.24</v>
       </c>
       <c r="H10" s="2">
         <v>0</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>83</v>
+      <c r="I10" s="7" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11" s="2">
         <v>4</v>
       </c>
       <c r="D11" s="8">
-        <v>85992536</v>
+        <v>25721866</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F11" s="9">
-        <v>7</v>
-      </c>
-      <c r="G11" s="5">
-        <v>0.28000000000000003</v>
+        <v>61</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="G11" s="6">
+        <v>0.47</v>
       </c>
       <c r="H11" s="2">
         <v>0</v>
       </c>
-      <c r="I11" s="2" t="s">
-        <v>84</v>
+      <c r="I11" s="7" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C12" s="2">
         <v>4</v>
       </c>
       <c r="D12" s="8">
-        <v>72764549</v>
+        <v>33055244</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F12" s="9">
-        <v>18</v>
-      </c>
-      <c r="G12" s="5">
-        <v>0.55000000000000004</v>
+        <v>61</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0.72</v>
       </c>
       <c r="H12" s="2">
         <v>0</v>
       </c>
-      <c r="I12" s="2" t="s">
-        <v>85</v>
+      <c r="I12" s="7" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C13" s="2">
         <v>4</v>
       </c>
       <c r="D13" s="8">
-        <v>45282573</v>
+        <v>90339235</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F13" s="9">
-        <v>24</v>
-      </c>
-      <c r="G13" s="5">
-        <v>0.85</v>
+        <v>127</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="G13" s="6">
+        <v>0.24</v>
       </c>
       <c r="H13" s="2">
         <v>0</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>86</v>
+      <c r="I13" s="7" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="2">
+        <v>4</v>
+      </c>
+      <c r="D14" s="8">
+        <v>72764549</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="2">
-        <v>4</v>
-      </c>
-      <c r="D14" s="8">
-        <v>59425241</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F14" s="9">
-        <v>7</v>
-      </c>
-      <c r="G14" s="5">
-        <v>0.28000000000000003</v>
+      <c r="F14" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="G14" s="6">
+        <v>0.47</v>
       </c>
       <c r="H14" s="2">
         <v>0</v>
       </c>
-      <c r="I14" s="2" t="s">
-        <v>87</v>
+      <c r="I14" s="7" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="2">
+        <v>4</v>
+      </c>
+      <c r="D15" s="8">
+        <v>45282573</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="2">
-        <v>4</v>
-      </c>
-      <c r="D15" s="8">
-        <v>32549606</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F15" s="9">
-        <v>18</v>
-      </c>
-      <c r="G15" s="5">
-        <v>0.55000000000000004</v>
+      <c r="F15" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="G15" s="6">
+        <v>0.72</v>
       </c>
       <c r="H15" s="2">
         <v>0</v>
       </c>
-      <c r="I15" s="2" t="s">
-        <v>88</v>
+      <c r="I15" s="7" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="2">
+        <v>4</v>
+      </c>
+      <c r="D16" s="8">
+        <v>85992536</v>
+      </c>
+      <c r="E16" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="2">
-        <v>4</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F16" s="9">
-        <v>24</v>
-      </c>
-      <c r="G16" s="5">
-        <v>0.85</v>
+      <c r="F16" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="G16" s="6">
+        <v>0.24</v>
       </c>
       <c r="H16" s="2">
         <v>0</v>
       </c>
-      <c r="I16" s="2" t="s">
-        <v>89</v>
+      <c r="I16" s="7" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C17" s="2">
         <v>4</v>
       </c>
       <c r="D17" s="8">
-        <v>90339235</v>
+        <v>32549606</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="F17" s="9">
-        <v>7</v>
-      </c>
-      <c r="G17" s="10">
-        <v>0.28000000000000003</v>
+        <v>47</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="G17" s="6">
+        <v>0.47</v>
       </c>
       <c r="H17" s="2">
         <v>0</v>
       </c>
-      <c r="I17" s="2" t="s">
-        <v>90</v>
+      <c r="I17" s="7" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C18" s="2">
         <v>4</v>
       </c>
-      <c r="D18" s="8">
-        <v>25721866</v>
+      <c r="D18" s="8" t="s">
+        <v>58</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="F18" s="9">
-        <v>18</v>
-      </c>
-      <c r="G18" s="5">
-        <v>0.55000000000000004</v>
+        <v>47</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="G18" s="6">
+        <v>0.72</v>
       </c>
       <c r="H18" s="2">
         <v>0</v>
       </c>
-      <c r="I18" s="2" t="s">
-        <v>91</v>
+      <c r="I18" s="7" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19" s="2">
         <v>4</v>
       </c>
       <c r="D19" s="8">
-        <v>33055244</v>
+        <v>59425241</v>
       </c>
       <c r="E19" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="G19" s="6">
+        <v>0.24</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0</v>
+      </c>
+      <c r="I19" s="7" t="s">
         <v>74</v>
-      </c>
-      <c r="F19" s="9">
-        <v>24</v>
-      </c>
-      <c r="G19" s="5">
-        <v>0.85</v>
-      </c>
-      <c r="H19" s="2">
-        <v>0</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1384,7 +1437,7 @@
         <v>23</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C20" s="2">
         <v>4</v>
@@ -1393,19 +1446,19 @@
         <v>74703631</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F20" s="9">
-        <v>23</v>
-      </c>
-      <c r="G20" s="5">
-        <v>1.75</v>
+        <v>48</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G20" s="6">
+        <v>1.49</v>
       </c>
       <c r="H20" s="2">
         <v>0</v>
       </c>
-      <c r="I20" s="2" t="s">
-        <v>93</v>
+      <c r="I20" s="7" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1413,7 +1466,7 @@
         <v>24</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C21" s="2">
         <v>4</v>
@@ -1422,19 +1475,19 @@
         <v>24459310</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F21" s="9">
-        <v>28</v>
-      </c>
-      <c r="G21" s="5">
-        <v>1.85</v>
+        <v>48</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G21" s="6">
+        <v>1.57</v>
       </c>
       <c r="H21" s="2">
         <v>0</v>
       </c>
-      <c r="I21" s="2" t="s">
-        <v>94</v>
+      <c r="I21" s="7" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1442,28 +1495,28 @@
         <v>25</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C22" s="2">
         <v>4</v>
       </c>
       <c r="D22" s="8">
-        <v>77031337</v>
+        <v>43875059</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="F22" s="9">
-        <v>18</v>
-      </c>
-      <c r="G22" s="5">
-        <v>0.55000000000000004</v>
+        <v>49</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="G22" s="6">
+        <v>1.49</v>
       </c>
       <c r="H22" s="2">
         <v>0</v>
       </c>
-      <c r="I22" s="2" t="s">
-        <v>95</v>
+      <c r="I22" s="7" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1471,789 +1524,931 @@
         <v>26</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C23" s="2">
         <v>4</v>
       </c>
       <c r="D23" s="8">
-        <v>43875059</v>
+        <v>38703336</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="F23" s="9">
-        <v>24</v>
-      </c>
-      <c r="G23" s="5">
-        <v>1.75</v>
+        <v>50</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G23" s="6">
+        <v>1.49</v>
       </c>
       <c r="H23" s="2">
         <v>0</v>
       </c>
-      <c r="I23" s="2" t="s">
-        <v>96</v>
+      <c r="I23" s="7" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>27</v>
+        <v>119</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C24" s="2">
         <v>4</v>
       </c>
-      <c r="D24" s="8">
-        <v>38703336</v>
+      <c r="D24" s="8" t="s">
+        <v>126</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="F24" s="9">
-        <v>23</v>
-      </c>
-      <c r="G24" s="5">
-        <v>1.75</v>
+        <v>154</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="G24" s="6">
+        <v>0.85</v>
       </c>
       <c r="H24" s="2">
         <v>0</v>
       </c>
-      <c r="I24" s="2" t="s">
-        <v>97</v>
+      <c r="I24" s="7" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>28</v>
+        <v>120</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C25" s="2">
         <v>4</v>
       </c>
       <c r="D25" s="8">
-        <v>44500664</v>
+        <v>97542115</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F25" s="9">
-        <v>6</v>
-      </c>
-      <c r="G25" s="5">
-        <v>1</v>
+        <v>154</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="G25" s="6">
+        <v>0.85</v>
       </c>
       <c r="H25" s="2">
         <v>0</v>
       </c>
-      <c r="I25" s="2" t="s">
-        <v>98</v>
+      <c r="I25" s="7" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C26" s="2">
         <v>4</v>
       </c>
       <c r="D26" s="8">
-        <v>28666261</v>
+        <v>44500664</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F26" s="9">
-        <v>7</v>
-      </c>
-      <c r="G26" s="5">
-        <v>1</v>
+        <v>149</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="G26" s="6">
+        <v>0.85</v>
       </c>
       <c r="H26" s="2">
         <v>0</v>
       </c>
-      <c r="I26" s="2" t="s">
-        <v>99</v>
+      <c r="I26" s="7" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C27" s="2">
         <v>4</v>
       </c>
       <c r="D27" s="8">
-        <v>97437944</v>
+        <v>28666261</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F27" s="9">
-        <v>6</v>
-      </c>
-      <c r="G27" s="5">
-        <v>1</v>
+        <v>149</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="G27" s="6">
+        <v>0.85</v>
       </c>
       <c r="H27" s="2">
         <v>0</v>
       </c>
-      <c r="I27" s="2" t="s">
-        <v>100</v>
+      <c r="I27" s="7" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C28" s="2">
         <v>4</v>
       </c>
-      <c r="D28" s="8" t="s">
-        <v>67</v>
+      <c r="D28" s="8">
+        <v>97437944</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F28" s="9">
-        <v>7</v>
-      </c>
-      <c r="G28" s="5">
-        <v>1</v>
+        <v>150</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="G28" s="6">
+        <v>0.85</v>
       </c>
       <c r="H28" s="2">
         <v>0</v>
       </c>
-      <c r="I28" s="2" t="s">
-        <v>101</v>
+      <c r="I28" s="7" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C29" s="2">
         <v>4</v>
       </c>
-      <c r="D29" s="8">
-        <v>15475355</v>
+      <c r="D29" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F29" s="9">
-        <v>6</v>
-      </c>
-      <c r="G29" s="5">
-        <v>1</v>
+        <v>150</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="G29" s="6">
+        <v>0.85</v>
       </c>
       <c r="H29" s="2">
         <v>0</v>
       </c>
-      <c r="I29" s="2" t="s">
-        <v>102</v>
+      <c r="I29" s="7" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C30" s="2">
         <v>4</v>
       </c>
       <c r="D30" s="8">
-        <v>88374842</v>
+        <v>15475355</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F30" s="9">
-        <v>7</v>
-      </c>
-      <c r="G30" s="5">
-        <v>1</v>
+        <v>151</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="G30" s="6">
+        <v>0.85</v>
       </c>
       <c r="H30" s="2">
         <v>0</v>
       </c>
-      <c r="I30" s="2" t="s">
-        <v>103</v>
+      <c r="I30" s="7" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C31" s="2">
         <v>4</v>
       </c>
       <c r="D31" s="8">
-        <v>75906062</v>
+        <v>88374842</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F31" s="9">
-        <v>6</v>
-      </c>
-      <c r="G31" s="5">
-        <v>0.28000000000000003</v>
+        <v>151</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="G31" s="6">
+        <v>0.85</v>
       </c>
       <c r="H31" s="2">
         <v>0</v>
       </c>
-      <c r="I31" s="2" t="s">
-        <v>104</v>
+      <c r="I31" s="7" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>35</v>
+        <v>113</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C32" s="2">
         <v>4</v>
       </c>
-      <c r="D32" s="8">
-        <v>69816024</v>
+      <c r="D32" s="8" t="s">
+        <v>118</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F32" s="9">
-        <v>10</v>
-      </c>
-      <c r="G32" s="5">
-        <v>0.55000000000000004</v>
+        <v>111</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="G32" s="6">
+        <v>0.47</v>
       </c>
       <c r="H32" s="2">
         <v>0</v>
       </c>
-      <c r="I32" s="2" t="s">
-        <v>105</v>
+      <c r="I32" s="7" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>36</v>
+        <v>114</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C33" s="2">
         <v>4</v>
       </c>
       <c r="D33" s="8">
-        <v>87369201</v>
+        <v>97609392</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F33" s="9">
-        <v>13</v>
-      </c>
-      <c r="G33" s="5">
-        <v>0.85</v>
+        <v>111</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="G33" s="6">
+        <v>0.72</v>
       </c>
       <c r="H33" s="2">
         <v>0</v>
       </c>
-      <c r="I33" s="2" t="s">
-        <v>106</v>
+      <c r="I33" s="7" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>37</v>
+        <v>112</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C34" s="2">
         <v>4</v>
       </c>
       <c r="D34" s="8">
-        <v>97210289</v>
+        <v>59785476</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F34" s="9">
-        <v>6</v>
-      </c>
-      <c r="G34" s="5">
-        <v>0.28000000000000003</v>
+        <v>111</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="G34" s="6">
+        <v>0.24</v>
       </c>
       <c r="H34" s="2">
         <v>0</v>
       </c>
-      <c r="I34" s="2" t="s">
-        <v>107</v>
+      <c r="I34" s="7" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>38</v>
+        <v>121</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C35" s="2">
         <v>4</v>
       </c>
       <c r="D35" s="8">
-        <v>64720586</v>
+        <v>38852609</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F35" s="9">
-        <v>10</v>
-      </c>
-      <c r="G35" s="5">
-        <v>0.55000000000000004</v>
+        <v>128</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="G35" s="6">
+        <v>0.47</v>
       </c>
       <c r="H35" s="2">
         <v>0</v>
       </c>
-      <c r="I35" s="2" t="s">
-        <v>108</v>
+      <c r="I35" s="7" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>39</v>
+        <v>122</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C36" s="2">
         <v>4</v>
       </c>
       <c r="D36" s="8">
-        <v>65385805</v>
+        <v>99938689</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F36" s="9">
-        <v>13</v>
-      </c>
-      <c r="G36" s="5">
-        <v>0.85</v>
+        <v>128</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="G36" s="6">
+        <v>0.72</v>
       </c>
       <c r="H36" s="2">
         <v>0</v>
       </c>
-      <c r="I36" s="2" t="s">
-        <v>109</v>
+      <c r="I36" s="7" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C37" s="2">
         <v>4</v>
       </c>
       <c r="D37" s="8">
-        <v>97210289</v>
+        <v>60616133</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="F37" s="9">
-        <v>6</v>
-      </c>
-      <c r="G37" s="5">
-        <v>0.28000000000000003</v>
+        <v>128</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="G37" s="6">
+        <v>0.24</v>
       </c>
       <c r="H37" s="2">
         <v>0</v>
       </c>
-      <c r="I37" s="2" t="s">
-        <v>120</v>
+      <c r="I37" s="7" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C38" s="2">
         <v>4</v>
       </c>
       <c r="D38" s="8">
-        <v>64720586</v>
+        <v>39285121</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="F38" s="9">
-        <v>10</v>
-      </c>
-      <c r="G38" s="5">
-        <v>0.55000000000000004</v>
+        <v>105</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="G38" s="6">
+        <v>0.47</v>
       </c>
       <c r="H38" s="2">
         <v>0</v>
       </c>
-      <c r="I38" s="2" t="s">
-        <v>121</v>
+      <c r="I38" s="7" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C39" s="2">
         <v>4</v>
       </c>
       <c r="D39" s="8">
-        <v>65385805</v>
+        <v>68087741</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="F39" s="9">
-        <v>13</v>
-      </c>
-      <c r="G39" s="5">
-        <v>0.85</v>
+        <v>105</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="G39" s="6">
+        <v>0.72</v>
       </c>
       <c r="H39" s="2">
         <v>0</v>
       </c>
-      <c r="I39" s="2" t="s">
-        <v>122</v>
+      <c r="I39" s="7" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>127</v>
+        <v>102</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C40" s="2">
         <v>4</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="F40" s="9">
-        <v>6</v>
-      </c>
-      <c r="G40" s="10">
-        <v>0.28000000000000003</v>
+        <v>105</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="G40" s="6">
+        <v>0.24</v>
       </c>
       <c r="H40" s="2">
         <v>0</v>
       </c>
-      <c r="I40" s="2" t="s">
-        <v>130</v>
+      <c r="I40" s="7" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>128</v>
+        <v>34</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C41" s="2">
         <v>4</v>
       </c>
-      <c r="D41" s="8" t="s">
-        <v>134</v>
+      <c r="D41" s="8">
+        <v>69816024</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="F41" s="9">
-        <v>10</v>
-      </c>
-      <c r="G41" s="10">
-        <v>0.55000000000000004</v>
+        <v>51</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="G41" s="6">
+        <v>0.47</v>
       </c>
       <c r="H41" s="2">
         <v>0</v>
       </c>
-      <c r="I41" s="2" t="s">
-        <v>131</v>
+      <c r="I41" s="7" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>129</v>
+        <v>35</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C42" s="2">
         <v>4</v>
       </c>
-      <c r="D42" s="8" t="s">
-        <v>135</v>
+      <c r="D42" s="8">
+        <v>87369201</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="F42" s="9">
-        <v>13</v>
-      </c>
-      <c r="G42" s="10">
-        <v>0.85</v>
+        <v>51</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="G42" s="6">
+        <v>0.72</v>
       </c>
       <c r="H42" s="2">
         <v>0</v>
       </c>
-      <c r="I42" s="2" t="s">
-        <v>132</v>
+      <c r="I42" s="7" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>123</v>
+        <v>33</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C43" s="2">
         <v>4</v>
       </c>
-      <c r="D43" s="8" t="s">
-        <v>125</v>
+      <c r="D43" s="8">
+        <v>75906062</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F43" s="9">
-        <v>5</v>
-      </c>
-      <c r="G43" s="10">
-        <v>0.25</v>
+        <v>51</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="G43" s="6">
+        <v>0.24</v>
       </c>
       <c r="H43" s="2">
         <v>0</v>
       </c>
-      <c r="I43" s="2" t="s">
-        <v>124</v>
+      <c r="I43" s="7" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C44" s="2">
         <v>4</v>
       </c>
       <c r="D44" s="8">
-        <v>78428095</v>
+        <v>64720586</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F44" s="9">
-        <v>7</v>
-      </c>
-      <c r="G44" s="5">
-        <v>0.28000000000000003</v>
+        <v>52</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="G44" s="6">
+        <v>0.47</v>
       </c>
       <c r="H44" s="2">
         <v>0</v>
       </c>
-      <c r="I44" s="2" t="s">
-        <v>110</v>
+      <c r="I44" s="7" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C45" s="2">
         <v>4</v>
       </c>
       <c r="D45" s="8">
-        <v>92989323</v>
+        <v>65385805</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F45" s="9">
-        <v>17</v>
-      </c>
-      <c r="G45" s="5">
-        <v>0.55000000000000004</v>
+        <v>52</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="G45" s="6">
+        <v>0.72</v>
       </c>
       <c r="H45" s="2">
         <v>0</v>
       </c>
-      <c r="I45" s="2" t="s">
-        <v>111</v>
+      <c r="I45" s="7" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C46" s="2">
         <v>4</v>
       </c>
       <c r="D46" s="8">
-        <v>83150019</v>
+        <v>97210289</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F46" s="9">
-        <v>23</v>
-      </c>
-      <c r="G46" s="5">
-        <v>0.85</v>
+        <v>52</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="G46" s="6">
+        <v>0.24</v>
       </c>
       <c r="H46" s="2">
         <v>0</v>
       </c>
-      <c r="I46" s="2" t="s">
-        <v>112</v>
+      <c r="I46" s="7" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C47" s="2">
         <v>4</v>
       </c>
       <c r="D47" s="8">
-        <v>59187767</v>
+        <v>92989323</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="F47" s="9">
-        <v>7</v>
-      </c>
-      <c r="G47" s="5">
-        <v>0.28000000000000003</v>
+        <v>152</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="G47" s="6">
+        <v>0.47</v>
       </c>
       <c r="H47" s="2">
         <v>0</v>
       </c>
-      <c r="I47" s="2" t="s">
-        <v>113</v>
+      <c r="I47" s="7" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>44</v>
+        <v>124</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C48" s="2">
         <v>4</v>
       </c>
       <c r="D48" s="8">
-        <v>91387284</v>
+        <v>59943846</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="F48" s="9">
-        <v>17</v>
-      </c>
-      <c r="G48" s="5">
-        <v>0.55000000000000004</v>
+        <v>152</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="G48" s="6">
+        <v>0.72</v>
       </c>
       <c r="H48" s="2">
         <v>0</v>
       </c>
-      <c r="I48" s="2" t="s">
-        <v>114</v>
+      <c r="I48" s="7" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C49" s="2">
         <v>4</v>
       </c>
       <c r="D49" s="8">
+        <v>83150019</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G49" s="6">
+        <v>0.72</v>
+      </c>
+      <c r="H49" s="2">
+        <v>0</v>
+      </c>
+      <c r="I49" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C50" s="2">
+        <v>4</v>
+      </c>
+      <c r="D50" s="8">
+        <v>49059947</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="G50" s="6">
+        <v>0.24</v>
+      </c>
+      <c r="H50" s="2">
+        <v>0</v>
+      </c>
+      <c r="I50" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C51" s="2">
+        <v>4</v>
+      </c>
+      <c r="D51" s="8">
+        <v>78428095</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="G51" s="6">
+        <v>0.24</v>
+      </c>
+      <c r="H51" s="2">
+        <v>0</v>
+      </c>
+      <c r="I51" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C52" s="2">
+        <v>4</v>
+      </c>
+      <c r="D52" s="8">
+        <v>91387284</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="G52" s="6">
+        <v>0.47</v>
+      </c>
+      <c r="H52" s="2">
+        <v>0</v>
+      </c>
+      <c r="I52" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C53" s="2">
+        <v>4</v>
+      </c>
+      <c r="D53" s="8">
         <v>32784264</v>
       </c>
-      <c r="E49" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="F49" s="9">
-        <v>23</v>
-      </c>
-      <c r="G49" s="5">
-        <v>0.85</v>
-      </c>
-      <c r="H49" s="2">
-        <v>0</v>
-      </c>
-      <c r="I49" s="2" t="s">
-        <v>115</v>
+      <c r="E53" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G53" s="6">
+        <v>0.72</v>
+      </c>
+      <c r="H53" s="2">
+        <v>0</v>
+      </c>
+      <c r="I53" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C54" s="2">
+        <v>4</v>
+      </c>
+      <c r="D54" s="8">
+        <v>59187767</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="G54" s="6">
+        <v>0.24</v>
+      </c>
+      <c r="H54" s="2">
+        <v>0</v>
+      </c>
+      <c r="I54" s="7" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="D43 D40:D42 D28" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>